<commit_message>
Pom implemented delete Contact with Organization
</commit_message>
<xml_diff>
--- a/SDET/testData/testScriptData.XLSX
+++ b/SDET/testData/testScriptData.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHEKHAR\git\sdet\SDET\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF63A0B-F89A-42B0-89DE-A9C920F493CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6A1DEC-0F0E-4483-9394-EBC73F9B8254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>testID</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>no Organization Found Message</t>
+  </si>
+  <si>
+    <t>No Contact Found !</t>
+  </si>
+  <si>
+    <t>no Contact Found Message</t>
   </si>
 </sst>
 </file>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5543B2FA-94BA-467C-AB20-33192642ABE8}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,9 +555,10 @@
     <col min="9" max="9" width="22.5703125" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,8 +592,11 @@
       <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -619,6 +629,9 @@
       </c>
       <c r="K2" t="s">
         <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>